<commit_message>
added xls results of spok and sparsification methods
</commit_message>
<xml_diff>
--- a/results_analysis/spok_chessboard_ttt.xlsx
+++ b/results_analysis/spok_chessboard_ttt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718986BF-7568-4115-8EB6-0972AB391E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7B3CDB-D0BA-4635-A862-2085F2BB6A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -989,7 +989,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,14 +1067,30 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="51"/>
+      <c r="D5" s="50">
+        <v>0.73281407035175905</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.85899497487437204</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.89614572864321596</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.92638190954773902</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.79865829145728595</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.51648743718593004</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.71262814070351799</v>
+      </c>
+      <c r="K5" s="51">
+        <v>0.91685929648241205</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -1082,14 +1098,30 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="53"/>
+      <c r="D6" s="52">
+        <v>0.87954271356783897</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.95092964824120596</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.87355778894472402</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.93480904522613095</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.88168341708542697</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.49936180904522598</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0.13148743718593001</v>
+      </c>
+      <c r="K6" s="53">
+        <v>0.94878391959799002</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1101,14 +1133,30 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="D7" s="54">
+        <v>0.88558793969849303</v>
+      </c>
+      <c r="E7" s="55">
+        <v>0.93197989949748705</v>
+      </c>
+      <c r="F7" s="55">
+        <v>0.58887939698492497</v>
+      </c>
+      <c r="G7" s="55">
+        <v>0.91926130653266303</v>
+      </c>
+      <c r="H7" s="55">
+        <v>0.91540703517587896</v>
+      </c>
+      <c r="I7" s="55">
+        <v>0.88766834170854303</v>
+      </c>
+      <c r="J7" s="55">
+        <v>0.667663316582915</v>
+      </c>
+      <c r="K7" s="56">
+        <v>0.91486934673366804</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -1116,14 +1164,30 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="53"/>
+      <c r="D8" s="52">
+        <v>0.91339698492462296</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.95953768844221099</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.88007537688442194</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0.94186432160804001</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0.95034170854271405</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.91879899497487405</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0.63125125628140699</v>
+      </c>
+      <c r="K8" s="53">
+        <v>0.95590954773869397</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1135,14 +1199,30 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="D9" s="54">
+        <v>0.552804020100503</v>
+      </c>
+      <c r="E9" s="55">
+        <v>0.512281407035176</v>
+      </c>
+      <c r="F9" s="55">
+        <v>0.89358291457286398</v>
+      </c>
+      <c r="G9" s="55">
+        <v>0.88551758793969904</v>
+      </c>
+      <c r="H9" s="55">
+        <v>0.92236683417085397</v>
+      </c>
+      <c r="I9" s="55">
+        <v>0.55281909547738695</v>
+      </c>
+      <c r="J9" s="55">
+        <v>0.129552763819095</v>
+      </c>
+      <c r="K9" s="56">
+        <v>0.88991959798995002</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -1150,14 +1230,30 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="53"/>
+      <c r="D10" s="52">
+        <v>0.552804020100503</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.94630150753768905</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.92666834170854295</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.94012060301507505</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.552804020100503</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0.552804020100503</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.121969849246231</v>
+      </c>
+      <c r="K10" s="53">
+        <v>8.1814070351758805E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -1169,14 +1265,30 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="D11" s="54">
+        <v>0.69760301507537703</v>
+      </c>
+      <c r="E11" s="55">
+        <v>0.55207035175879404</v>
+      </c>
+      <c r="F11" s="55">
+        <v>0.86878391959798995</v>
+      </c>
+      <c r="G11" s="55">
+        <v>0.77828643216080395</v>
+      </c>
+      <c r="H11" s="55">
+        <v>0.55283919597990006</v>
+      </c>
+      <c r="I11" s="55">
+        <v>0.618879396984925</v>
+      </c>
+      <c r="J11" s="55">
+        <v>0.636241206030151</v>
+      </c>
+      <c r="K11" s="56">
+        <v>0.55067839195979895</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -1184,14 +1296,30 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="53"/>
+      <c r="D12" s="52">
+        <v>0.57516080402010095</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.93445226130653303</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.85137688442211101</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0.90069346733668298</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.936914572864322</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0.942125628140704</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.65072361809045198</v>
+      </c>
+      <c r="K12" s="53">
+        <v>0.94266834170854297</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D13" s="15"/>
@@ -1537,7 +1665,7 @@
   <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1545,13 +1673,17 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -1680,22 +1812,54 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="26"/>
+      <c r="D5" s="27">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="E5" s="26">
+        <v>1024.001</v>
+      </c>
+      <c r="F5" s="27">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="G5" s="26">
+        <v>1024.001</v>
+      </c>
+      <c r="H5" s="27">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="I5" s="26">
+        <v>1024.001</v>
+      </c>
+      <c r="J5" s="12">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="K5" s="26">
+        <v>1024.001</v>
+      </c>
+      <c r="L5" s="12">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="M5" s="26">
+        <v>1024.001</v>
+      </c>
+      <c r="N5" s="12">
+        <v>-7.8125E-3</v>
+      </c>
+      <c r="O5" s="26">
+        <v>1024.001</v>
+      </c>
+      <c r="P5" s="27">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>1024.001</v>
+      </c>
+      <c r="R5" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="S5" s="26">
+        <v>1024.001</v>
+      </c>
     </row>
     <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -1703,22 +1867,54 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
+      <c r="D6" s="30">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="E6" s="28">
+        <v>1024.001</v>
+      </c>
+      <c r="F6" s="29">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="G6" s="28">
+        <v>1024.001</v>
+      </c>
+      <c r="H6" s="28">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="I6" s="28">
+        <v>1024.001</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="28">
+        <v>1024.001</v>
+      </c>
+      <c r="L6" s="18">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="M6" s="28">
+        <v>1024.001</v>
+      </c>
+      <c r="N6" s="13">
+        <v>-3.90625E-3</v>
+      </c>
+      <c r="O6" s="28">
+        <v>1024.001</v>
+      </c>
+      <c r="P6" s="30">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="Q6" s="28">
+        <v>1024.001</v>
+      </c>
+      <c r="R6" s="28">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S6" s="28">
+        <v>1024.001</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1730,22 +1926,54 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="13"/>
+      <c r="D7" s="29">
+        <v>0.999</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0.4</v>
+      </c>
+      <c r="G7" s="13">
+        <v>1</v>
+      </c>
+      <c r="H7" s="29">
+        <v>0.7</v>
+      </c>
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
+      <c r="J7" s="29">
+        <v>0.999</v>
+      </c>
+      <c r="K7" s="13">
+        <v>1</v>
+      </c>
+      <c r="L7" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="M7" s="13">
+        <v>1</v>
+      </c>
+      <c r="N7" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="O7" s="28">
+        <v>1</v>
+      </c>
+      <c r="P7" s="29">
+        <v>0.7</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>1</v>
+      </c>
+      <c r="R7" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="S7" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -1753,22 +1981,54 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="13"/>
+      <c r="D8" s="29">
+        <v>0.999</v>
+      </c>
+      <c r="E8" s="13">
+        <v>1</v>
+      </c>
+      <c r="F8" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="29">
+        <v>0.99</v>
+      </c>
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="K8" s="13">
+        <v>1</v>
+      </c>
+      <c r="L8" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="M8" s="13">
+        <v>1</v>
+      </c>
+      <c r="N8" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="O8" s="28">
+        <v>1</v>
+      </c>
+      <c r="P8" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>1</v>
+      </c>
+      <c r="R8" s="18">
+        <v>0.6</v>
+      </c>
+      <c r="S8" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1780,22 +2040,54 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="13"/>
+      <c r="D9" s="30">
+        <v>16</v>
+      </c>
+      <c r="E9" s="28">
+        <v>512.0009765625</v>
+      </c>
+      <c r="F9" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="28">
+        <v>512.0009765625</v>
+      </c>
+      <c r="H9" s="30">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="I9" s="13">
+        <v>8.7890625E-3</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="28">
+        <v>64.0009765625</v>
+      </c>
+      <c r="L9" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="M9" s="13">
+        <v>8.0009765625</v>
+      </c>
+      <c r="N9" s="30">
+        <v>4</v>
+      </c>
+      <c r="O9" s="30">
+        <v>1.0009765625</v>
+      </c>
+      <c r="P9" s="30">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>32.0009765625</v>
+      </c>
+      <c r="R9" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="S9" s="13">
+        <v>32.0009765625</v>
+      </c>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -1803,22 +2095,54 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="13"/>
+      <c r="D10" s="28">
+        <v>8</v>
+      </c>
+      <c r="E10" s="28">
+        <v>256.0009765625</v>
+      </c>
+      <c r="F10" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="18">
+        <v>2.9296875E-3</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
+      <c r="I10" s="28">
+        <v>4.8828125E-3</v>
+      </c>
+      <c r="J10" s="28">
+        <v>1</v>
+      </c>
+      <c r="K10" s="28">
+        <v>256.0009765625</v>
+      </c>
+      <c r="L10" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="M10" s="28">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="N10" s="28">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="O10" s="30">
+        <v>0.2509765625</v>
+      </c>
+      <c r="P10" s="13">
+        <v>256</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>4.8828125E-3</v>
+      </c>
+      <c r="R10" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="S10" s="13">
+        <v>512.0009765625</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -1830,22 +2154,54 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
+      <c r="D11" s="28">
+        <v>1</v>
+      </c>
+      <c r="E11" s="28">
+        <v>64.0009765625</v>
+      </c>
+      <c r="F11" s="28">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="G11" s="28">
+        <v>1.0009765625</v>
+      </c>
+      <c r="H11" s="30">
+        <v>3.125E-2</v>
+      </c>
+      <c r="I11" s="28">
+        <v>1.0009765625</v>
+      </c>
+      <c r="J11" s="30">
+        <v>6.25E-2</v>
+      </c>
+      <c r="K11" s="30">
+        <v>2.0009765625</v>
+      </c>
+      <c r="L11" s="13">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="M11" s="18">
+        <v>1.0009765625</v>
+      </c>
+      <c r="N11" s="28">
+        <v>-1024</v>
+      </c>
+      <c r="O11" s="13">
+        <v>16.0009765625</v>
+      </c>
+      <c r="P11" s="30">
+        <v>0.125</v>
+      </c>
+      <c r="Q11" s="28">
+        <v>1024.0009765625</v>
+      </c>
+      <c r="R11" s="28">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="S11" s="28">
+        <v>1.0009765625</v>
+      </c>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -1853,22 +2209,54 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="13"/>
+      <c r="D12" s="30">
+        <v>64</v>
+      </c>
+      <c r="E12" s="28">
+        <v>512.0009765625</v>
+      </c>
+      <c r="F12" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="30">
+        <v>256.0009765625</v>
+      </c>
+      <c r="H12" s="30">
+        <v>4</v>
+      </c>
+      <c r="I12" s="13">
+        <v>8.0009765625</v>
+      </c>
+      <c r="J12" s="30">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="K12" s="30">
+        <v>0.2509765625</v>
+      </c>
+      <c r="L12" s="30">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M12" s="28">
+        <v>128.0009765625</v>
+      </c>
+      <c r="N12" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="O12" s="28">
+        <v>16.0009765625</v>
+      </c>
+      <c r="P12" s="13">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>512.0009765625</v>
+      </c>
+      <c r="R12" s="30">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="S12" s="13">
+        <v>32.0009765625</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
@@ -2183,7 +2571,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2261,14 +2649,30 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="51"/>
+      <c r="D5" s="50">
+        <v>0.66145391703342205</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.85554731647876003</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.874976028308319</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.92021452337051901</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.79673033468209797</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.50337306593620501</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.67495774804290298</v>
+      </c>
+      <c r="K5" s="51">
+        <v>0.90979055414532195</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -2276,14 +2680,30 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="53"/>
+      <c r="D6" s="52">
+        <v>0.84751415424798204</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.93519984972459202</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.83316732768172896</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.91512247259133706</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.87625972200749402</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.48301099685228499</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0.12396064200561099</v>
+      </c>
+      <c r="K6" s="53">
+        <v>0.93066835328441699</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -2295,14 +2715,30 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="D7" s="54">
+        <v>0.88111308525096299</v>
+      </c>
+      <c r="E7" s="55">
+        <v>0.92470915793543795</v>
+      </c>
+      <c r="F7" s="55">
+        <v>0.58191393567722804</v>
+      </c>
+      <c r="G7" s="55">
+        <v>0.91186865242386095</v>
+      </c>
+      <c r="H7" s="55">
+        <v>0.90606982205795605</v>
+      </c>
+      <c r="I7" s="55">
+        <v>0.872810046758974</v>
+      </c>
+      <c r="J7" s="55">
+        <v>0.67657861276957398</v>
+      </c>
+      <c r="K7" s="56">
+        <v>0.90495419309234504</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -2310,14 +2746,30 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="53"/>
+      <c r="D8" s="52">
+        <v>0.89782030235713906</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.94617091257474195</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.87301920002151101</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0.92118863598355405</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0.93477213813653204</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.89366809916172396</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0.63964529249503999</v>
+      </c>
+      <c r="K8" s="53">
+        <v>0.94069676749406195</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -2329,14 +2781,30 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="D9" s="54">
+        <v>0.54427267028896997</v>
+      </c>
+      <c r="E9" s="55">
+        <v>0.56529316403551499</v>
+      </c>
+      <c r="F9" s="55">
+        <v>0.88937440572383397</v>
+      </c>
+      <c r="G9" s="55">
+        <v>0.87881604448444695</v>
+      </c>
+      <c r="H9" s="55">
+        <v>0.91638803122031098</v>
+      </c>
+      <c r="I9" s="55">
+        <v>0.54428555274492996</v>
+      </c>
+      <c r="J9" s="55">
+        <v>0.126614410433007</v>
+      </c>
+      <c r="K9" s="56">
+        <v>0.884376137437488</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -2344,14 +2812,30 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="53"/>
+      <c r="D10" s="52">
+        <v>0.54427267028896997</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.92775580665819202</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.92110118937444296</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.92136457376826097</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.54427267028896997</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0.54427267028896997</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.119803620387363</v>
+      </c>
+      <c r="K10" s="53">
+        <v>8.3606505973758197E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -2363,14 +2847,30 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="D11" s="54">
+        <v>0.65810394449929799</v>
+      </c>
+      <c r="E11" s="55">
+        <v>0.54400319845731104</v>
+      </c>
+      <c r="F11" s="55">
+        <v>0.84593690356705697</v>
+      </c>
+      <c r="G11" s="55">
+        <v>0.77066495198041796</v>
+      </c>
+      <c r="H11" s="55">
+        <v>0.54472991310849195</v>
+      </c>
+      <c r="I11" s="55">
+        <v>0.61017109351678001</v>
+      </c>
+      <c r="J11" s="55">
+        <v>0.62895927506179305</v>
+      </c>
+      <c r="K11" s="56">
+        <v>0.54258052405090795</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -2378,14 +2878,30 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="53"/>
+      <c r="D12" s="52">
+        <v>0.57138156444123001</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.91859889801586703</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.77967286404993097</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0.81780634923334306</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.91770254011103003</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0.92336653202955599</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.613483646121322</v>
+      </c>
+      <c r="K12" s="53">
+        <v>0.92480689877219602</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D13" s="15"/>
@@ -2811,7 +3327,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2889,14 +3405,30 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="51"/>
+      <c r="D5" s="50">
+        <v>0.73281502849503999</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.86061364574731603</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.89617372900664805</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.92689717559553697</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.806121790736679</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.54049999999999998</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.713574229691877</v>
+      </c>
+      <c r="K5" s="51">
+        <v>0.917132731034765</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -2904,14 +3436,30 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="53"/>
+      <c r="D6" s="52">
+        <v>0.87954271356783897</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.95095603980350196</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.873558130058807</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.93480918104033695</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.88238555361951498</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.52449999999999997</v>
+      </c>
+      <c r="J6" s="14">
+        <v>0.134984631352042</v>
+      </c>
+      <c r="K6" s="53">
+        <v>0.94881366178026305</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -2923,14 +3471,30 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="D7" s="54">
+        <v>0.88753196367163401</v>
+      </c>
+      <c r="E7" s="55">
+        <v>0.93215433180025697</v>
+      </c>
+      <c r="F7" s="55">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="G7" s="55">
+        <v>0.91938856624962695</v>
+      </c>
+      <c r="H7" s="55">
+        <v>0.91564050632911398</v>
+      </c>
+      <c r="I7" s="55">
+        <v>0.887817053771911</v>
+      </c>
+      <c r="J7" s="55">
+        <v>0.69908333333333295</v>
+      </c>
+      <c r="K7" s="56">
+        <v>0.91494112048278198</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -2938,14 +3502,30 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="53"/>
+      <c r="D8" s="52">
+        <v>0.91344953906847604</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.95954416813701104</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0.880256250884632</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0.94187352945622005</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0.95034224201184003</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.91879899497487405</v>
+      </c>
+      <c r="J8" s="14">
+        <v>0.68497254118821804</v>
+      </c>
+      <c r="K8" s="53">
+        <v>0.95590954773869397</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -2957,14 +3537,30 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="D9" s="54">
+        <v>0.55928608223993204</v>
+      </c>
+      <c r="E9" s="55">
+        <v>0.80750137892995</v>
+      </c>
+      <c r="F9" s="55">
+        <v>0.89499642236532795</v>
+      </c>
+      <c r="G9" s="55">
+        <v>0.88570816457697799</v>
+      </c>
+      <c r="H9" s="55">
+        <v>0.92257332800008096</v>
+      </c>
+      <c r="I9" s="55">
+        <v>0.55928608223993204</v>
+      </c>
+      <c r="J9" s="55">
+        <v>0.14266161297115201</v>
+      </c>
+      <c r="K9" s="56">
+        <v>0.89301355578727803</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -2972,14 +3568,30 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="53"/>
+      <c r="D10" s="52">
+        <v>0.55928608223993204</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.94632921835541695</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0.92678928500657498</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.94013997446752695</v>
+      </c>
+      <c r="H10" s="14">
+        <v>0.55928608223993204</v>
+      </c>
+      <c r="I10" s="14">
+        <v>0.55928608223993204</v>
+      </c>
+      <c r="J10" s="14">
+        <v>0.131225806451613</v>
+      </c>
+      <c r="K10" s="53">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -2991,14 +3603,30 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="D11" s="54">
+        <v>0.69843434343434296</v>
+      </c>
+      <c r="E11" s="55">
+        <v>0.55748136476577204</v>
+      </c>
+      <c r="F11" s="55">
+        <v>0.86934398424249104</v>
+      </c>
+      <c r="G11" s="55">
+        <v>0.77939361702127696</v>
+      </c>
+      <c r="H11" s="55">
+        <v>0.55964970758461896</v>
+      </c>
+      <c r="I11" s="55">
+        <v>0.63388709677419397</v>
+      </c>
+      <c r="J11" s="55">
+        <v>0.644620967741935</v>
+      </c>
+      <c r="K11" s="56">
+        <v>0.55789218508530103</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -3006,14 +3634,30 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="53"/>
+      <c r="D12" s="52">
+        <v>0.59423429428428598</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.93448447918714195</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0.85137742846518005</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0.90069346733668298</v>
+      </c>
+      <c r="H12" s="14">
+        <v>0.93692538274287296</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0.94212886000705298</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.65226222780089704</v>
+      </c>
+      <c r="K12" s="53">
+        <v>0.94266834170854297</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D13" s="15"/>
@@ -3439,7 +4083,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3517,14 +4161,30 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="51"/>
+      <c r="D5" s="50">
+        <v>5.35346034748162E-2</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2.27932501473826E-2</v>
+      </c>
+      <c r="F5" s="12">
+        <v>3.6055955976468601E-2</v>
+      </c>
+      <c r="G5" s="12">
+        <v>2.8592728466769E-2</v>
+      </c>
+      <c r="H5" s="12">
+        <v>2.0452093431476699E-2</v>
+      </c>
+      <c r="I5" s="12">
+        <v>3.1825695009188699E-2</v>
+      </c>
+      <c r="J5" s="12">
+        <v>6.1295699383232302E-2</v>
+      </c>
+      <c r="K5" s="51">
+        <v>2.7832442013410098E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -3532,14 +4192,30 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="53"/>
+      <c r="D6" s="52">
+        <v>4.5807551827140899E-2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>3.1368400942304898E-2</v>
+      </c>
+      <c r="F6" s="14">
+        <v>5.1473918095921299E-2</v>
+      </c>
+      <c r="G6" s="14">
+        <v>3.0657108834655802E-2</v>
+      </c>
+      <c r="H6" s="14">
+        <v>2.5874184990942201E-2</v>
+      </c>
+      <c r="I6" s="14">
+        <v>3.2039547105791502E-2</v>
+      </c>
+      <c r="J6" s="14">
+        <v>1.3439764981078199E-2</v>
+      </c>
+      <c r="K6" s="53">
+        <v>3.5348105697645502E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -3551,14 +4227,30 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="D7" s="54">
+        <v>2.5846196050730501E-2</v>
+      </c>
+      <c r="E7" s="55">
+        <v>2.9524315957331199E-2</v>
+      </c>
+      <c r="F7" s="55">
+        <v>2.9317914302692299E-2</v>
+      </c>
+      <c r="G7" s="55">
+        <v>2.7614200507041099E-2</v>
+      </c>
+      <c r="H7" s="55">
+        <v>2.8800998825402602E-2</v>
+      </c>
+      <c r="I7" s="55">
+        <v>2.6898618777444101E-2</v>
+      </c>
+      <c r="J7" s="55">
+        <v>2.2353245658621901E-2</v>
+      </c>
+      <c r="K7" s="56">
+        <v>2.85845441418194E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -3566,14 +4258,30 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="53"/>
+      <c r="D8" s="52">
+        <v>3.0452390900084201E-2</v>
+      </c>
+      <c r="E8" s="14">
+        <v>3.3206835434398299E-2</v>
+      </c>
+      <c r="F8" s="14">
+        <v>2.67511249173366E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <v>3.4678832771024203E-2</v>
+      </c>
+      <c r="H8" s="14">
+        <v>3.1515174825504103E-2</v>
+      </c>
+      <c r="I8" s="14">
+        <v>3.7072495039982001E-2</v>
+      </c>
+      <c r="J8" s="14">
+        <v>2.3762238360220098E-2</v>
+      </c>
+      <c r="K8" s="53">
+        <v>3.21405986146008E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -3585,14 +4293,30 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="D9" s="54">
+        <v>3.6443637578204797E-2</v>
+      </c>
+      <c r="E9" s="55">
+        <v>7.6231099173373604E-2</v>
+      </c>
+      <c r="F9" s="55">
+        <v>2.4943009462193699E-2</v>
+      </c>
+      <c r="G9" s="55">
+        <v>3.6370627674693998E-2</v>
+      </c>
+      <c r="H9" s="55">
+        <v>2.7289649151684602E-2</v>
+      </c>
+      <c r="I9" s="55">
+        <v>3.6446492182573398E-2</v>
+      </c>
+      <c r="J9" s="55">
+        <v>8.90786730583552E-3</v>
+      </c>
+      <c r="K9" s="56">
+        <v>3.6983887807488298E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -3600,14 +4324,30 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="53"/>
+      <c r="D10" s="52">
+        <v>3.6443637578204797E-2</v>
+      </c>
+      <c r="E10" s="14">
+        <v>4.0812454059811903E-2</v>
+      </c>
+      <c r="F10" s="14">
+        <v>2.6132961740805101E-2</v>
+      </c>
+      <c r="G10" s="14">
+        <v>4.75070486438329E-2</v>
+      </c>
+      <c r="H10" s="14">
+        <v>3.6443637578204797E-2</v>
+      </c>
+      <c r="I10" s="14">
+        <v>3.6443637578204797E-2</v>
+      </c>
+      <c r="J10" s="14">
+        <v>1.03987847967268E-2</v>
+      </c>
+      <c r="K10" s="53">
+        <v>6.42852927834E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -3619,14 +4359,30 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="D11" s="54">
+        <v>5.5007512346806203E-2</v>
+      </c>
+      <c r="E11" s="55">
+        <v>3.5977542224307102E-2</v>
+      </c>
+      <c r="F11" s="55">
+        <v>5.2812020035553499E-2</v>
+      </c>
+      <c r="G11" s="55">
+        <v>2.1836217179628001E-2</v>
+      </c>
+      <c r="H11" s="55">
+        <v>3.4949073483213099E-2</v>
+      </c>
+      <c r="I11" s="55">
+        <v>4.1619176116102802E-2</v>
+      </c>
+      <c r="J11" s="55">
+        <v>3.6938418877778101E-2</v>
+      </c>
+      <c r="K11" s="56">
+        <v>3.4856101628455503E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -3634,14 +4390,30 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="53"/>
+      <c r="D12" s="52">
+        <v>3.0098417947317602E-2</v>
+      </c>
+      <c r="E12" s="14">
+        <v>3.0655573717985898E-2</v>
+      </c>
+      <c r="F12" s="14">
+        <v>8.3258504947795603E-2</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0.110605692389009</v>
+      </c>
+      <c r="H12" s="14">
+        <v>2.9991417424895399E-2</v>
+      </c>
+      <c r="I12" s="14">
+        <v>3.2701670485702598E-2</v>
+      </c>
+      <c r="J12" s="14">
+        <v>4.6620028147920503E-2</v>
+      </c>
+      <c r="K12" s="53">
+        <v>3.2183670966720798E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D13" s="15"/>
@@ -4067,7 +4839,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4075,13 +4847,11 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -4145,14 +4915,30 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="D5" s="18">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="18">
+        <v>151</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1000</v>
+      </c>
+      <c r="H5" s="18">
+        <v>57</v>
+      </c>
+      <c r="I5" s="18">
+        <v>999</v>
+      </c>
+      <c r="J5" s="18">
+        <v>1000</v>
+      </c>
+      <c r="K5" s="18">
+        <v>1000</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -4160,14 +4946,30 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="D6" s="18">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1000</v>
+      </c>
+      <c r="F6" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G6" s="18">
+        <v>1000</v>
+      </c>
+      <c r="H6" s="18">
+        <v>162</v>
+      </c>
+      <c r="I6" s="18">
+        <v>998</v>
+      </c>
+      <c r="J6" s="18">
+        <v>8</v>
+      </c>
+      <c r="K6" s="18">
+        <v>528</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -4179,14 +4981,30 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="D7" s="18">
+        <v>279</v>
+      </c>
+      <c r="E7" s="18">
+        <v>751</v>
+      </c>
+      <c r="F7" s="18">
+        <v>17</v>
+      </c>
+      <c r="G7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="H7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="I7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="18">
+        <v>1000</v>
+      </c>
+      <c r="K7" s="18">
+        <v>1000</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -4194,14 +5012,30 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="D8" s="18">
+        <v>810</v>
+      </c>
+      <c r="E8" s="18">
+        <v>257</v>
+      </c>
+      <c r="F8" s="18">
+        <v>223</v>
+      </c>
+      <c r="G8" s="18">
+        <v>256</v>
+      </c>
+      <c r="H8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="I8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="18">
+        <v>1000</v>
+      </c>
+      <c r="K8" s="18">
+        <v>1000</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -4213,14 +5047,30 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="D9" s="18">
+        <v>8</v>
+      </c>
+      <c r="E9" s="18">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="18">
+        <v>280</v>
+      </c>
+      <c r="G9" s="18">
+        <v>999</v>
+      </c>
+      <c r="H9" s="18">
+        <v>1000</v>
+      </c>
+      <c r="I9" s="18">
+        <v>8</v>
+      </c>
+      <c r="J9" s="18">
+        <v>8</v>
+      </c>
+      <c r="K9" s="18">
+        <v>1000</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -4228,14 +5078,30 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="D10" s="18">
+        <v>8</v>
+      </c>
+      <c r="E10" s="18">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="18">
+        <v>64</v>
+      </c>
+      <c r="G10" s="18">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="18">
+        <v>8</v>
+      </c>
+      <c r="I10" s="18">
+        <v>8</v>
+      </c>
+      <c r="J10" s="18">
+        <v>8</v>
+      </c>
+      <c r="K10" s="18">
+        <v>1000</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -4247,14 +5113,30 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="D11" s="18">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="18">
+        <v>8</v>
+      </c>
+      <c r="F11" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G11" s="18">
+        <v>102</v>
+      </c>
+      <c r="H11" s="18">
+        <v>8</v>
+      </c>
+      <c r="I11" s="18">
+        <v>994</v>
+      </c>
+      <c r="J11" s="18">
+        <v>999</v>
+      </c>
+      <c r="K11" s="18">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -4262,14 +5144,30 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="D12" s="18">
+        <v>469</v>
+      </c>
+      <c r="E12" s="18">
+        <v>1000</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G12" s="18">
+        <v>1000</v>
+      </c>
+      <c r="H12" s="18">
+        <v>1000</v>
+      </c>
+      <c r="I12" s="18">
+        <v>1000</v>
+      </c>
+      <c r="J12" s="18">
+        <v>1000</v>
+      </c>
+      <c r="K12" s="18">
+        <v>893</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
@@ -4457,7 +5355,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4535,14 +5433,30 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="D5" s="18">
+        <v>975.56915075376901</v>
+      </c>
+      <c r="E5" s="18">
+        <v>148.74650251256301</v>
+      </c>
+      <c r="F5" s="18">
+        <v>998.39813065326598</v>
+      </c>
+      <c r="G5" s="18">
+        <v>993.72931155778895</v>
+      </c>
+      <c r="H5" s="18">
+        <v>52.331949748743703</v>
+      </c>
+      <c r="I5" s="18">
+        <v>968.59942713567796</v>
+      </c>
+      <c r="J5" s="18">
+        <v>978.40555778894498</v>
+      </c>
+      <c r="K5" s="18">
+        <v>997.08672864321602</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -4550,14 +5464,30 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="D6" s="18">
+        <v>997.87590452261304</v>
+      </c>
+      <c r="E6" s="18">
+        <v>996.27868844221098</v>
+      </c>
+      <c r="F6" s="18">
+        <v>998.13011557789002</v>
+      </c>
+      <c r="G6" s="18">
+        <v>997.50503015075401</v>
+      </c>
+      <c r="H6" s="18">
+        <v>157.857115577889</v>
+      </c>
+      <c r="I6" s="18">
+        <v>967.72046231155798</v>
+      </c>
+      <c r="J6" s="18">
+        <v>8.4474170854271406</v>
+      </c>
+      <c r="K6" s="18">
+        <v>515.234522613065</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -4569,14 +5499,30 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="D7" s="18">
+        <v>270.37907537688397</v>
+      </c>
+      <c r="E7" s="18">
+        <v>727.16397989949803</v>
+      </c>
+      <c r="F7" s="18">
+        <v>16.638653266331701</v>
+      </c>
+      <c r="G7" s="18">
+        <v>996.98887437185897</v>
+      </c>
+      <c r="H7" s="18">
+        <v>998.04639698492497</v>
+      </c>
+      <c r="I7" s="18">
+        <v>999.57740201005004</v>
+      </c>
+      <c r="J7" s="18">
+        <v>998.14918090452295</v>
+      </c>
+      <c r="K7" s="18">
+        <v>998.041236180905</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -4584,14 +5530,30 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="D8" s="18">
+        <v>700.36879899497501</v>
+      </c>
+      <c r="E8" s="18">
+        <v>258.20204522613102</v>
+      </c>
+      <c r="F8" s="18">
+        <v>211.30160804020099</v>
+      </c>
+      <c r="G8" s="18">
+        <v>244.16710050251299</v>
+      </c>
+      <c r="H8" s="18">
+        <v>995.07459798995001</v>
+      </c>
+      <c r="I8" s="18">
+        <v>999.59997487437204</v>
+      </c>
+      <c r="J8" s="18">
+        <v>997.87113065326605</v>
+      </c>
+      <c r="K8" s="18">
+        <v>993.65949246231196</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -4603,14 +5565,30 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="D9" s="18">
+        <v>7.9998844221105498</v>
+      </c>
+      <c r="E9" s="18">
+        <v>990.97296984924606</v>
+      </c>
+      <c r="F9" s="18">
+        <v>297.61526633165801</v>
+      </c>
+      <c r="G9" s="18">
+        <v>984.75113065326605</v>
+      </c>
+      <c r="H9" s="18">
+        <v>975.160452261307</v>
+      </c>
+      <c r="I9" s="18">
+        <v>7.9998844221105498</v>
+      </c>
+      <c r="J9" s="18">
+        <v>8.4948693467336707</v>
+      </c>
+      <c r="K9" s="18">
+        <v>984.887542713568</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -4618,14 +5596,30 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="D10" s="18">
+        <v>7.9998844221105498</v>
+      </c>
+      <c r="E10" s="18">
+        <v>982.69625628140705</v>
+      </c>
+      <c r="F10" s="18">
+        <v>63.386643216080401</v>
+      </c>
+      <c r="G10" s="18">
+        <v>986.66068341708603</v>
+      </c>
+      <c r="H10" s="18">
+        <v>7.9998844221105498</v>
+      </c>
+      <c r="I10" s="18">
+        <v>7.9998844221105498</v>
+      </c>
+      <c r="J10" s="18">
+        <v>7.9998844221105498</v>
+      </c>
+      <c r="K10" s="18">
+        <v>997.79246733668299</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -4637,14 +5631,30 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="D11" s="18">
+        <v>969.68030653266305</v>
+      </c>
+      <c r="E11" s="18">
+        <v>32.473608040201</v>
+      </c>
+      <c r="F11" s="18">
+        <v>990.37382914572902</v>
+      </c>
+      <c r="G11" s="18">
+        <v>171.01741206030201</v>
+      </c>
+      <c r="H11" s="18">
+        <v>8.2701105527638195</v>
+      </c>
+      <c r="I11" s="18">
+        <v>993.53903517587901</v>
+      </c>
+      <c r="J11" s="18">
+        <v>995.96821105527602</v>
+      </c>
+      <c r="K11" s="18">
+        <v>11.528788944723599</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -4652,14 +5662,30 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="D12" s="18">
+        <v>276.82482914572898</v>
+      </c>
+      <c r="E12" s="18">
+        <v>994.35435678392003</v>
+      </c>
+      <c r="F12" s="18">
+        <v>994.07357286432205</v>
+      </c>
+      <c r="G12" s="18">
+        <v>932.52224120603</v>
+      </c>
+      <c r="H12" s="18">
+        <v>996.42538190954804</v>
+      </c>
+      <c r="I12" s="18">
+        <v>997.40818090452296</v>
+      </c>
+      <c r="J12" s="18">
+        <v>864.33894974874397</v>
+      </c>
+      <c r="K12" s="18">
+        <v>722.70235175879395</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
@@ -4847,7 +5873,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4925,14 +5951,30 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="D5" s="18">
+        <v>116.199890520466</v>
+      </c>
+      <c r="E5" s="18">
+        <v>5.5858576212242497</v>
+      </c>
+      <c r="F5" s="18">
+        <v>23.469522385936099</v>
+      </c>
+      <c r="G5" s="18">
+        <v>48.826309729379602</v>
+      </c>
+      <c r="H5" s="18">
+        <v>3.8835622832401699</v>
+      </c>
+      <c r="I5" s="18">
+        <v>112.188119537422</v>
+      </c>
+      <c r="J5" s="18">
+        <v>126.104107690286</v>
+      </c>
+      <c r="K5" s="18">
+        <v>36.926654025718697</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -4940,14 +5982,30 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="D6" s="18">
+        <v>29.103818628643701</v>
+      </c>
+      <c r="E6" s="18">
+        <v>41.113668609107201</v>
+      </c>
+      <c r="F6" s="18">
+        <v>26.4706792007979</v>
+      </c>
+      <c r="G6" s="18">
+        <v>35.103522509529697</v>
+      </c>
+      <c r="H6" s="18">
+        <v>4.5819880145621896</v>
+      </c>
+      <c r="I6" s="18">
+        <v>111.99000730825</v>
+      </c>
+      <c r="J6" s="18">
+        <v>5.8124617282447799</v>
+      </c>
+      <c r="K6" s="18">
+        <v>26.413245733859799</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -4959,14 +6017,30 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="D7" s="18">
+        <v>10.538867793071301</v>
+      </c>
+      <c r="E7" s="18">
+        <v>37.761776755305</v>
+      </c>
+      <c r="F7" s="18">
+        <v>2.5628862963752299</v>
+      </c>
+      <c r="G7" s="18">
+        <v>37.142702060034999</v>
+      </c>
+      <c r="H7" s="18">
+        <v>31.008552568541301</v>
+      </c>
+      <c r="I7" s="18">
+        <v>10.288174805130099</v>
+      </c>
+      <c r="J7" s="18">
+        <v>21.4708791057821</v>
+      </c>
+      <c r="K7" s="18">
+        <v>31.0429963846472</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -4974,14 +6048,30 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="D8" s="18">
+        <v>102.849366176651</v>
+      </c>
+      <c r="E8" s="18">
+        <v>7.8303124055734799</v>
+      </c>
+      <c r="F8" s="18">
+        <v>10.0476033892748</v>
+      </c>
+      <c r="G8" s="18">
+        <v>15.601682330925501</v>
+      </c>
+      <c r="H8" s="18">
+        <v>47.292522498809198</v>
+      </c>
+      <c r="I8" s="18">
+        <v>10.2879802146426</v>
+      </c>
+      <c r="J8" s="18">
+        <v>21.674770543077599</v>
+      </c>
+      <c r="K8" s="18">
+        <v>52.036744733642401</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -4993,14 +6083,30 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="D9" s="18">
+        <v>1.7792446350428801E-2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>64.302637020608898</v>
+      </c>
+      <c r="F9" s="18">
+        <v>14.802167287506</v>
+      </c>
+      <c r="G9" s="18">
+        <v>86.105855734520006</v>
+      </c>
+      <c r="H9" s="18">
+        <v>110.63653855916699</v>
+      </c>
+      <c r="I9" s="18">
+        <v>1.7792446350428801E-2</v>
+      </c>
+      <c r="J9" s="18">
+        <v>1.33750790263009</v>
+      </c>
+      <c r="K9" s="18">
+        <v>85.581756396399101</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -5008,14 +6114,30 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="D10" s="18">
+        <v>1.7792446350428801E-2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>92.370418199137603</v>
+      </c>
+      <c r="F10" s="18">
+        <v>1.3447173881280301</v>
+      </c>
+      <c r="G10" s="18">
+        <v>78.417224394120396</v>
+      </c>
+      <c r="H10" s="18">
+        <v>1.7792446350428801E-2</v>
+      </c>
+      <c r="I10" s="18">
+        <v>1.7792446350428801E-2</v>
+      </c>
+      <c r="J10" s="18">
+        <v>1.7792446350428801E-2</v>
+      </c>
+      <c r="K10" s="18">
+        <v>34.524802829248998</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -5027,14 +6149,30 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="D11" s="18">
+        <v>100.649888197102</v>
+      </c>
+      <c r="E11" s="18">
+        <v>17.803907928608702</v>
+      </c>
+      <c r="F11" s="18">
+        <v>78.334305184101197</v>
+      </c>
+      <c r="G11" s="18">
+        <v>92.237333822680199</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0.87325354822884604</v>
+      </c>
+      <c r="I11" s="18">
+        <v>35.8017234178403</v>
+      </c>
+      <c r="J11" s="18">
+        <v>43.418294435842597</v>
+      </c>
+      <c r="K11" s="18">
+        <v>3.9532269727650302</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -5042,14 +6180,30 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="D12" s="18">
+        <v>126.995775157167</v>
+      </c>
+      <c r="E12" s="18">
+        <v>50.193623602634702</v>
+      </c>
+      <c r="F12" s="18">
+        <v>58.638738131392998</v>
+      </c>
+      <c r="G12" s="18">
+        <v>220.03422235724199</v>
+      </c>
+      <c r="H12" s="18">
+        <v>44.805009673984699</v>
+      </c>
+      <c r="I12" s="18">
+        <v>39.468085192813803</v>
+      </c>
+      <c r="J12" s="18">
+        <v>321.13476051678902</v>
+      </c>
+      <c r="K12" s="18">
+        <v>146.19977503908601</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
@@ -5237,7 +6391,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5315,14 +6469,30 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1</v>
+      </c>
+      <c r="H5" s="18">
+        <v>1</v>
+      </c>
+      <c r="I5" s="18">
+        <v>1</v>
+      </c>
+      <c r="J5" s="18">
+        <v>1</v>
+      </c>
+      <c r="K5" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -5330,14 +6500,30 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
+      <c r="D6" s="18">
+        <v>5</v>
+      </c>
+      <c r="E6" s="18">
+        <v>5</v>
+      </c>
+      <c r="F6" s="18">
+        <v>10</v>
+      </c>
+      <c r="G6" s="18">
+        <v>8</v>
+      </c>
+      <c r="H6" s="18">
+        <v>2</v>
+      </c>
+      <c r="I6" s="18">
+        <v>6</v>
+      </c>
+      <c r="J6" s="18">
+        <v>6</v>
+      </c>
+      <c r="K6" s="18">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -5349,14 +6535,30 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+      <c r="E7" s="18">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1</v>
+      </c>
+      <c r="G7" s="18">
+        <v>1</v>
+      </c>
+      <c r="H7" s="18">
+        <v>1</v>
+      </c>
+      <c r="I7" s="18">
+        <v>1</v>
+      </c>
+      <c r="J7" s="18">
+        <v>1</v>
+      </c>
+      <c r="K7" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -5364,14 +6566,30 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="D8" s="18">
+        <v>3</v>
+      </c>
+      <c r="E8" s="18">
+        <v>8</v>
+      </c>
+      <c r="F8" s="18">
+        <v>3</v>
+      </c>
+      <c r="G8" s="18">
+        <v>6</v>
+      </c>
+      <c r="H8" s="18">
+        <v>4</v>
+      </c>
+      <c r="I8" s="18">
+        <v>8</v>
+      </c>
+      <c r="J8" s="18">
+        <v>6</v>
+      </c>
+      <c r="K8" s="18">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -5383,14 +6601,30 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
+      <c r="D9" s="18">
+        <v>1</v>
+      </c>
+      <c r="E9" s="18">
+        <v>1</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1</v>
+      </c>
+      <c r="G9" s="18">
+        <v>1</v>
+      </c>
+      <c r="H9" s="18">
+        <v>1</v>
+      </c>
+      <c r="I9" s="18">
+        <v>1</v>
+      </c>
+      <c r="J9" s="18">
+        <v>1</v>
+      </c>
+      <c r="K9" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -5398,14 +6632,30 @@
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
+      <c r="D10" s="18">
+        <v>3</v>
+      </c>
+      <c r="E10" s="18">
+        <v>2</v>
+      </c>
+      <c r="F10" s="18">
+        <v>4</v>
+      </c>
+      <c r="G10" s="18">
+        <v>4</v>
+      </c>
+      <c r="H10" s="18">
+        <v>5</v>
+      </c>
+      <c r="I10" s="18">
+        <v>4</v>
+      </c>
+      <c r="J10" s="18">
+        <v>10</v>
+      </c>
+      <c r="K10" s="18">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -5417,14 +6667,30 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+      <c r="E11" s="18">
+        <v>1</v>
+      </c>
+      <c r="F11" s="18">
+        <v>1</v>
+      </c>
+      <c r="G11" s="18">
+        <v>1</v>
+      </c>
+      <c r="H11" s="18">
+        <v>1</v>
+      </c>
+      <c r="I11" s="18">
+        <v>1</v>
+      </c>
+      <c r="J11" s="18">
+        <v>1</v>
+      </c>
+      <c r="K11" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -5432,14 +6698,30 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
+      <c r="D12" s="18">
+        <v>5</v>
+      </c>
+      <c r="E12" s="18">
+        <v>10</v>
+      </c>
+      <c r="F12" s="18">
+        <v>4</v>
+      </c>
+      <c r="G12" s="18">
+        <v>6</v>
+      </c>
+      <c r="H12" s="18">
+        <v>9</v>
+      </c>
+      <c r="I12" s="18">
+        <v>2</v>
+      </c>
+      <c r="J12" s="18">
+        <v>4</v>
+      </c>
+      <c r="K12" s="18">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
@@ -5627,7 +6909,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5641,8 +6923,9 @@
     <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5758,19 +7041,45 @@
       <c r="C5" s="20">
         <v>1</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="37"/>
+      <c r="D5" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="36">
+        <v>1024</v>
+      </c>
+      <c r="G5" s="36">
+        <v>512</v>
+      </c>
+      <c r="H5" s="36">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I5" s="36">
+        <v>32</v>
+      </c>
+      <c r="J5" s="36">
+        <v>2</v>
+      </c>
+      <c r="K5" s="36">
+        <v>0.8</v>
+      </c>
+      <c r="L5" s="36">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="M5" s="32">
+        <v>1</v>
+      </c>
+      <c r="N5" s="34">
+        <v>-0.5</v>
+      </c>
+      <c r="O5" s="36">
+        <v>3.125E-2</v>
+      </c>
+      <c r="P5" s="37">
+        <v>6.25E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -5778,19 +7087,45 @@
       <c r="C6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="42"/>
+      <c r="D6" s="39">
+        <v>32</v>
+      </c>
+      <c r="E6" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F6" s="28">
+        <v>512</v>
+      </c>
+      <c r="G6" s="28">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="H6" s="28">
+        <v>2</v>
+      </c>
+      <c r="I6" s="13">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J6" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="28">
+        <v>0.6</v>
+      </c>
+      <c r="L6" s="28">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="M6" s="31">
+        <v>128</v>
+      </c>
+      <c r="N6" s="13">
+        <v>-2</v>
+      </c>
+      <c r="O6" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="P6" s="42">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -5802,19 +7137,45 @@
       <c r="C7" s="20">
         <v>1</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="41"/>
+      <c r="D7" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="18">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F7" s="28">
+        <v>512</v>
+      </c>
+      <c r="G7" s="30">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H7" s="28">
+        <v>2.6</v>
+      </c>
+      <c r="I7" s="28">
+        <v>16</v>
+      </c>
+      <c r="J7" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="K7" s="18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L7" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="M7" s="31">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="N7" s="13">
+        <v>-9.765625E-4</v>
+      </c>
+      <c r="O7" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="P7" s="41">
+        <v>3.125E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -5822,19 +7183,45 @@
       <c r="C8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="41"/>
+      <c r="D8" s="39">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="E8" s="30">
+        <v>0.125</v>
+      </c>
+      <c r="F8" s="13">
+        <v>16</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="18">
+        <v>2.6</v>
+      </c>
+      <c r="I8" s="30">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="J8" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="K8" s="28">
+        <v>0.4</v>
+      </c>
+      <c r="L8" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="M8" s="31">
+        <v>0.25</v>
+      </c>
+      <c r="N8" s="13">
+        <v>-0.125</v>
+      </c>
+      <c r="O8" s="30">
+        <v>0.25</v>
+      </c>
+      <c r="P8" s="41">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -5846,19 +7233,45 @@
       <c r="C9" s="20">
         <v>1</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="43"/>
+      <c r="D9" s="39">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E9" s="28">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="F9" s="30">
+        <v>8</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0.125</v>
+      </c>
+      <c r="H9" s="18">
+        <v>1</v>
+      </c>
+      <c r="I9" s="28">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="J9" s="31">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="K9" s="18">
+        <v>3</v>
+      </c>
+      <c r="L9" s="28">
+        <v>256</v>
+      </c>
+      <c r="M9" s="13">
+        <v>16</v>
+      </c>
+      <c r="N9" s="13">
+        <v>6.25E-2</v>
+      </c>
+      <c r="O9" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="P9" s="43">
+        <v>3.125E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -5866,19 +7279,45 @@
       <c r="C10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="43"/>
+      <c r="D10" s="38">
+        <v>4</v>
+      </c>
+      <c r="E10" s="28">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="F10" s="28">
+        <v>32</v>
+      </c>
+      <c r="G10" s="18">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H10" s="18">
+        <v>1</v>
+      </c>
+      <c r="I10" s="28">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="J10" s="31">
+        <v>4</v>
+      </c>
+      <c r="K10" s="28">
+        <v>2.4</v>
+      </c>
+      <c r="L10" s="28">
+        <v>512</v>
+      </c>
+      <c r="M10" s="31">
+        <v>9.765625E-4</v>
+      </c>
+      <c r="N10" s="18">
+        <v>32</v>
+      </c>
+      <c r="O10" s="29">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="P10" s="43">
+        <v>7.8125E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -5890,19 +7329,45 @@
       <c r="C11" s="21">
         <v>1</v>
       </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="43"/>
+      <c r="D11" s="38">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="E11" s="28">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F11" s="13">
+        <v>4</v>
+      </c>
+      <c r="G11" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="H11" s="18">
+        <v>2.6</v>
+      </c>
+      <c r="I11" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="18">
+        <v>64</v>
+      </c>
+      <c r="K11" s="28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L11" s="28">
+        <v>32</v>
+      </c>
+      <c r="M11" s="31">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="N11" s="18">
+        <v>6.25E-2</v>
+      </c>
+      <c r="O11" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="P11" s="43">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
@@ -5910,19 +7375,45 @@
       <c r="C12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="49"/>
+      <c r="D12" s="40">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0.125</v>
+      </c>
+      <c r="F12" s="47">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G12" s="45">
+        <v>256</v>
+      </c>
+      <c r="H12" s="46">
+        <v>2.4</v>
+      </c>
+      <c r="I12" s="33">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J12" s="33">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="K12" s="46">
+        <v>2</v>
+      </c>
+      <c r="L12" s="47">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M12" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="14">
+        <v>1.953125E-3</v>
+      </c>
+      <c r="O12" s="44">
+        <v>3.125E-2</v>
+      </c>
+      <c r="P12" s="49">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>

</xml_diff>